<commit_message>
No tinc clar si funciona...
He tret resultats, però només per règim estacionari, perquè per no estacionari no obtinc res. A més, els coeficients tampoc em donen resultats coherents :(.
</commit_message>
<xml_diff>
--- a/Square cylinder/Coefficients.xlsx
+++ b/Square cylinder/Coefficients.xlsx
@@ -363,15 +363,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -382,7 +382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -393,7 +393,7 @@
         <v>28.485199999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -404,7 +404,7 @@
         <v>4.3063099999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>30</v>
       </c>
@@ -424,26 +424,76 @@
         <v>11.473100000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>-2.9719700000000002E-2</v>
+      </c>
+      <c r="G5">
+        <v>4.1525100000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>-2.4142299999999998E-2</v>
+      </c>
+      <c r="G6">
+        <v>2.82355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E7">
         <v>10</v>
       </c>
-      <c r="F5">
+      <c r="F7">
         <v>-0.22930200000000001</v>
       </c>
-      <c r="G5">
+      <c r="G7">
         <v>13.1638</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E6">
+      <c r="H7">
+        <v>-1.5935499999999998E-2</v>
+      </c>
+      <c r="I7">
+        <v>1.8965799999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8">
         <v>30</v>
       </c>
-      <c r="F6">
+      <c r="F8">
         <v>-4.2999700000000002E-3</v>
       </c>
-      <c r="G6">
+      <c r="G8">
         <v>2.0407999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="F9">
+        <v>1.6830700000000001E-3</v>
+      </c>
+      <c r="G9">
+        <v>1.3654200000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>1.3698499999999999E-3</v>
+      </c>
+      <c r="G10">
+        <v>2.1631300000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>